<commit_message>
show delete and edit
</commit_message>
<xml_diff>
--- a/RESTfulBlogApp/restful routes.xlsx
+++ b/RESTfulBlogApp/restful routes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651960DA-9AAA-45DF-9DEC-4088C1174260}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0FE3F3-A982-4E44-97A8-788FA73DD127}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -98,6 +98,30 @@
   </si>
   <si>
     <t>Delete a particular dog, then redirect somewhere</t>
+  </si>
+  <si>
+    <t>Mongoose Method</t>
+  </si>
+  <si>
+    <t>Dog.find()</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Dog.create()</t>
+  </si>
+  <si>
+    <t>Dog.findById()</t>
+  </si>
+  <si>
+    <t>Dog.findById</t>
+  </si>
+  <si>
+    <t>Dog.findByIdAndUpdate()</t>
+  </si>
+  <si>
+    <t>Dog.findByIdAndRemove()</t>
   </si>
 </sst>
 </file>
@@ -162,10 +186,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D9"/>
+  <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,9 +482,10 @@
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="44.88671875" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -472,8 +498,11 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -486,8 +515,11 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -500,8 +532,11 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -514,8 +549,11 @@
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -528,8 +566,11 @@
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -542,8 +583,11 @@
       <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -556,8 +600,11 @@
       <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -569,6 +616,9 @@
       </c>
       <c r="D9" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>